<commit_message>
add measurement for BR1 & 2
</commit_message>
<xml_diff>
--- a/through-wall-wire.xlsx
+++ b/through-wall-wire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilson/Documents/github/renovation-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08D4E67-B9DF-124A-A78D-D7805CFC7A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53453413-BEF6-7649-B47F-A15A7DA1E511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" xr2:uid="{70A70C4D-9B03-A84C-8FAD-8D30E20DAC9D}"/>
+    <workbookView xWindow="6180" yWindow="6940" windowWidth="33600" windowHeight="19120" xr2:uid="{70A70C4D-9B03-A84C-8FAD-8D30E20DAC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="through-wall-wire" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>W01</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>＊ 數字為線所經過掣位的次序</t>
+  </si>
+  <si>
+    <t>線長 （cm)</t>
   </si>
 </sst>
 </file>
@@ -358,6 +361,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,9 +373,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,7 +690,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,7 +698,7 @@
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -707,24 +710,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="7" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -736,7 +739,9 @@
       <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>41</v>
       </c>
@@ -775,82 +780,85 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="7">
+        <f>275+205+205+226+53</f>
+        <v>964</v>
+      </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
       <c r="O5" s="1">
         <v>1</v>
       </c>
@@ -859,258 +867,258 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
         <v>2</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="1">
         <v>3</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="1">
         <v>1</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="1">
         <v>1</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="1">
         <v>1</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
       <c r="K10" s="1">
         <v>2</v>
       </c>
-      <c r="L10" s="10"/>
+      <c r="L10" s="7"/>
       <c r="M10" s="1">
         <v>1</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>2</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="1">
         <v>1</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="1">
         <v>1</v>
       </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
       <c r="N14" s="1">
         <v>1</v>
       </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="11" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="3">
         <f>COUNT(E3:E14)</f>
         <v>2</v>

</xml_diff>